<commit_message>
Allow emails to be sent to email based on admission number
</commit_message>
<xml_diff>
--- a/Student_Attendance_Input/FSD_Class_1A.xlsx
+++ b/Student_Attendance_Input/FSD_Class_1A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewj\Documents\UiPath\Project\Student_Attendance_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A8E694-9621-4C5D-BDD1-495240093D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E8BF8-9366-4E3D-AC0A-A5A45C00CDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{93CD790B-59D2-4617-94E0-276DB9D5BB6C}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>Payton Richmond</t>
   </si>
   <si>
-    <t>2401404E</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Jeffrey Allen</t>
   </si>
   <si>
-    <t>2401411W</t>
-  </si>
-  <si>
     <t>Riley Reynolds</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>Shay Fry</t>
   </si>
   <si>
-    <t>3414131B</t>
-  </si>
-  <si>
     <t>Jacoby Rosas</t>
   </si>
   <si>
@@ -249,6 +240,15 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>E401404E</t>
+  </si>
+  <si>
+    <t>L401411W</t>
+  </si>
+  <si>
+    <t>N414131B</t>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,12 +688,12 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -746,1149 +746,1149 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feature to send excel summary report to lecturer through email, attached one excel file contains multiple sheets for each class/subject
</commit_message>
<xml_diff>
--- a/Student_Attendance_Input/FSD_Class_1A.xlsx
+++ b/Student_Attendance_Input/FSD_Class_1A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewj\Documents\UiPath\Project\Student_Attendance_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E8BF8-9366-4E3D-AC0A-A5A45C00CDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E822AF-E35C-4D30-9C2A-1DECF7DFFD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{93CD790B-59D2-4617-94E0-276DB9D5BB6C}"/>
   </bookViews>
@@ -654,7 +654,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removed a paragraph in a word doc because we aren't showing table in the warning pdf letter
</commit_message>
<xml_diff>
--- a/Student_Attendance_Input/FSD_Class_1A.xlsx
+++ b/Student_Attendance_Input/FSD_Class_1A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewj\Documents\UiPath\Project\Student_Attendance_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E822AF-E35C-4D30-9C2A-1DECF7DFFD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF1C62-F1B5-4CC7-9E56-A39E31FDD4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{93CD790B-59D2-4617-94E0-276DB9D5BB6C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="70">
   <si>
     <t>Class:</t>
   </si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>m</t>
   </si>
   <si>
     <t>Name</t>
@@ -654,7 +651,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +690,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -746,7 +743,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1196,7 +1193,7 @@
         <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -1355,7 +1352,7 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
@@ -1746,7 +1743,7 @@
         <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>

</xml_diff>